<commit_message>
Fixing errors. Updating classification.
</commit_message>
<xml_diff>
--- a/ANALYSIS/DATA/luscinia/bad_files_2020.xlsx
+++ b/ANALYSIS/DATA/luscinia/bad_files_2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssmeele/ownCloud/Simeon/MPI AB/PhD thesis/Chapter II/voice_paper/ANALYSIS/DATA/luscinia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29DFD68-7961-C747-A368-B0D84FB5427A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602A317A-920A-3A47-9CCC-090AFD553DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="1502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="1512">
   <si>
     <t>file_end</t>
   </si>
@@ -4537,6 +4537,36 @@
   </si>
   <si>
     <t>13_110538-1</t>
+  </si>
+  <si>
+    <t>08_102624-9</t>
+  </si>
+  <si>
+    <t>13_160716-8</t>
+  </si>
+  <si>
+    <t>16_075656-3</t>
+  </si>
+  <si>
+    <t>03_142030-2</t>
+  </si>
+  <si>
+    <t>06_152146-9</t>
+  </si>
+  <si>
+    <t>05_163428-10</t>
+  </si>
+  <si>
+    <t>05_163428-8</t>
+  </si>
+  <si>
+    <t>17_082744-2</t>
+  </si>
+  <si>
+    <t>05_163428-7</t>
+  </si>
+  <si>
+    <t>02_144820-7</t>
   </si>
 </sst>
 </file>
@@ -4931,10 +4961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1504"/>
+  <dimension ref="A1:C1514"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1479" workbookViewId="0">
-      <selection activeCell="C1504" sqref="C1504"/>
+    <sheetView tabSelected="1" topLeftCell="A1492" workbookViewId="0">
+      <selection activeCell="A1514" sqref="A1514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13961,6 +13991,66 @@
       </c>
       <c r="B1504">
         <v>1</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1505" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B1505" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1505" s="1"/>
+    </row>
+    <row r="1506" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1506" s="1" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B1506">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1507" s="1" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1508" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1509" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1510" s="1" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B1510">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1511" s="1" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1512" s="1" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1513" s="1" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1514" s="1" t="s">
+        <v>1511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>